<commit_message>
use case textuel interroger transformation en excel en cours
</commit_message>
<xml_diff>
--- a/documents/analyse_uml/usecase_textuel/use_case_administrer/Creeradmin.xlsx
+++ b/documents/analyse_uml/usecase_textuel/use_case_administrer/Creeradmin.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\Quideance\documents\analyse_uml\usecase_textuel\use_case_administrer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1D6F4B2E-5FB1-40E9-8E23-CFF561ADFB07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47B2DABD-55BF-4DA4-949A-6606E546BD16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="27600" windowHeight="15630" xr2:uid="{47DE18DC-D680-4772-96B6-916E44320A59}"/>
   </bookViews>
@@ -755,8 +755,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{639F26A4-991A-4628-A62A-CA800A4679FC}">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
use case textuel modifier
</commit_message>
<xml_diff>
--- a/documents/analyse_uml/usecase_textuel/use_case_administrer/Creeradmin.xlsx
+++ b/documents/analyse_uml/usecase_textuel/use_case_administrer/Creeradmin.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\Quideance\documents\analyse_uml\usecase_textuel\use_case_administrer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47B2DABD-55BF-4DA4-949A-6606E546BD16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF3CBB66-F2D9-4D33-88AC-6B3C27A36DB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="27600" windowHeight="15630" xr2:uid="{47DE18DC-D680-4772-96B6-916E44320A59}"/>
   </bookViews>
@@ -263,6 +263,9 @@
     </r>
   </si>
   <si>
+    <t>6) Quideance enregistre le formulaire</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
@@ -272,7 +275,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>E2) Erreur serveur</t>
+      <t>E2) L'enregistrement ne se valide pas</t>
     </r>
     <r>
       <rPr>
@@ -298,9 +301,6 @@
       </rPr>
       <t>On sort du USE CASE sur un échec</t>
     </r>
-  </si>
-  <si>
-    <t>6) Quideance enregistre le formulaire</t>
   </si>
 </sst>
 </file>
@@ -755,8 +755,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{639F26A4-991A-4628-A62A-CA800A4679FC}">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -842,13 +842,13 @@
       </c>
       <c r="C9" s="1"/>
     </row>
-    <row r="10" spans="1:4" ht="75.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="91.5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -903,5 +903,6 @@
     <mergeCell ref="D1:D2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
verification des séquentiels de admin
</commit_message>
<xml_diff>
--- a/documents/analyse_uml/usecase_textuel/use_case_administrer/Creeradmin.xlsx
+++ b/documents/analyse_uml/usecase_textuel/use_case_administrer/Creeradmin.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\Quideance\documents\analyse_uml\usecase_textuel\use_case_administrer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\symfony\Quideance\documents\analyse_uml\usecase_textuel\use_case_administrer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF3CBB66-F2D9-4D33-88AC-6B3C27A36DB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABB46521-7D84-48E9-B57E-F4100B7DC0C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="27600" windowHeight="15630" xr2:uid="{47DE18DC-D680-4772-96B6-916E44320A59}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{47DE18DC-D680-4772-96B6-916E44320A59}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -753,10 +753,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{639F26A4-991A-4628-A62A-CA800A4679FC}">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="A13" sqref="A13:A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -863,41 +863,6 @@
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="D1:D2"/>

</xml_diff>